<commit_message>
added refinery, officer patrols rows
</commit_message>
<xml_diff>
--- a/src/main/resources/Shift Report Template.xlsx
+++ b/src/main/resources/Shift Report Template.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Sheet2" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Team Leaders Report'!$A$1:$E$88</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Team Leaders Report'!$A$1:$E$90</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="188">
   <si>
     <t xml:space="preserve">Shift Report</t>
   </si>
@@ -297,13 +297,22 @@
     <t xml:space="preserve">Hiremasters</t>
   </si>
   <si>
-    <t xml:space="preserve">Car Park Patrols </t>
+    <t xml:space="preserve">Car Park</t>
   </si>
   <si>
     <t xml:space="preserve">Factory Road Warehouse</t>
   </si>
   <si>
-    <t xml:space="preserve">Perimeter Patrol</t>
+    <t xml:space="preserve">Perimeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refinery</t>
   </si>
   <si>
     <t xml:space="preserve">Comments / Observations:</t>
@@ -484,9 +493,6 @@
   </si>
   <si>
     <t xml:space="preserve">Ali Kawasr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">Not Reported </t>
@@ -913,7 +919,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1099,6 +1105,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1331,10 +1349,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T1048576"/>
+  <dimension ref="A1:T12162"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B74" activeCellId="0" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.96484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2339,14 +2357,16 @@
       <c r="S75" s="5"/>
       <c r="T75" s="5"/>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B76" s="47"/>
-      <c r="C76" s="47"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
+      <c r="B76" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
+      <c r="E76" s="49"/>
       <c r="M76" s="5"/>
       <c r="N76" s="5"/>
       <c r="O76" s="5"/>
@@ -2356,12 +2376,16 @@
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="48"/>
-      <c r="B77" s="48"/>
-      <c r="C77" s="48"/>
-      <c r="D77" s="48"/>
-      <c r="E77" s="48"/>
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C77" s="46"/>
+      <c r="D77" s="46"/>
+      <c r="E77" s="46"/>
       <c r="M77" s="5"/>
       <c r="N77" s="5"/>
       <c r="O77" s="5"/>
@@ -2372,11 +2396,13 @@
       <c r="T77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="48"/>
-      <c r="B78" s="48"/>
-      <c r="C78" s="48"/>
-      <c r="D78" s="48"/>
-      <c r="E78" s="48"/>
+      <c r="A78" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" s="50"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
       <c r="M78" s="5"/>
       <c r="N78" s="5"/>
       <c r="O78" s="5"/>
@@ -2386,12 +2412,12 @@
       <c r="S78" s="5"/>
       <c r="T78" s="5"/>
     </row>
-    <row r="79" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="48"/>
-      <c r="B79" s="48"/>
-      <c r="C79" s="48"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="51"/>
+      <c r="B79" s="51"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
+      <c r="E79" s="51"/>
       <c r="M79" s="5"/>
       <c r="N79" s="5"/>
       <c r="O79" s="5"/>
@@ -2402,11 +2428,11 @@
       <c r="T79" s="5"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="48"/>
-      <c r="B80" s="48"/>
-      <c r="C80" s="48"/>
-      <c r="D80" s="48"/>
-      <c r="E80" s="48"/>
+      <c r="A80" s="51"/>
+      <c r="B80" s="51"/>
+      <c r="C80" s="51"/>
+      <c r="D80" s="51"/>
+      <c r="E80" s="51"/>
       <c r="M80" s="5"/>
       <c r="N80" s="5"/>
       <c r="O80" s="5"/>
@@ -2416,12 +2442,12 @@
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="48"/>
-      <c r="B81" s="48"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="48"/>
-      <c r="E81" s="48"/>
+    <row r="81" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="51"/>
+      <c r="B81" s="51"/>
+      <c r="C81" s="51"/>
+      <c r="D81" s="51"/>
+      <c r="E81" s="51"/>
       <c r="M81" s="5"/>
       <c r="N81" s="5"/>
       <c r="O81" s="5"/>
@@ -2431,14 +2457,12 @@
       <c r="S81" s="5"/>
       <c r="T81" s="5"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="51"/>
+      <c r="B82" s="51"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="51"/>
+      <c r="E82" s="51"/>
       <c r="M82" s="5"/>
       <c r="N82" s="5"/>
       <c r="O82" s="5"/>
@@ -2449,19 +2473,11 @@
       <c r="T82" s="5"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="B83" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C83" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="D83" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="E83" s="49"/>
+      <c r="A83" s="51"/>
+      <c r="B83" s="51"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="51"/>
+      <c r="E83" s="51"/>
       <c r="M83" s="5"/>
       <c r="N83" s="5"/>
       <c r="O83" s="5"/>
@@ -2472,11 +2488,13 @@
       <c r="T83" s="5"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="50"/>
-      <c r="B84" s="50"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
-      <c r="E84" s="50"/>
+      <c r="A84" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
       <c r="M84" s="5"/>
       <c r="N84" s="5"/>
       <c r="O84" s="5"/>
@@ -2487,11 +2505,19 @@
       <c r="T84" s="5"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="50"/>
-      <c r="B85" s="50"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
-      <c r="E85" s="50"/>
+      <c r="A85" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B85" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D85" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="52"/>
       <c r="M85" s="5"/>
       <c r="N85" s="5"/>
       <c r="O85" s="5"/>
@@ -2502,11 +2528,11 @@
       <c r="T85" s="5"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="50"/>
-      <c r="B86" s="50"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="50"/>
+      <c r="A86" s="53"/>
+      <c r="B86" s="53"/>
+      <c r="C86" s="53"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="53"/>
       <c r="M86" s="5"/>
       <c r="N86" s="5"/>
       <c r="O86" s="5"/>
@@ -2517,11 +2543,11 @@
       <c r="T86" s="5"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="51"/>
-      <c r="B87" s="50"/>
-      <c r="C87" s="51"/>
-      <c r="D87" s="51"/>
-      <c r="E87" s="51"/>
+      <c r="A87" s="53"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="53"/>
+      <c r="E87" s="53"/>
       <c r="M87" s="5"/>
       <c r="N87" s="5"/>
       <c r="O87" s="5"/>
@@ -2531,18 +2557,12 @@
       <c r="S87" s="5"/>
       <c r="T87" s="5"/>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="B88" s="16"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="52" t="s">
-        <v>100</v>
-      </c>
-      <c r="E88" s="53" t="n">
-        <v>0.75</v>
-      </c>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="53"/>
+      <c r="B88" s="53"/>
+      <c r="C88" s="53"/>
+      <c r="D88" s="53"/>
+      <c r="E88" s="53"/>
       <c r="M88" s="5"/>
       <c r="N88" s="5"/>
       <c r="O88" s="5"/>
@@ -2552,18 +2572,12 @@
       <c r="S88" s="5"/>
       <c r="T88" s="5"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="B89" s="54"/>
-      <c r="C89" s="33"/>
-      <c r="D89" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="E89" s="53" t="n">
-        <v>0.75</v>
-      </c>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="54"/>
+      <c r="B89" s="53"/>
+      <c r="C89" s="54"/>
+      <c r="D89" s="54"/>
+      <c r="E89" s="54"/>
       <c r="M89" s="5"/>
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
@@ -2573,7 +2587,18 @@
       <c r="S89" s="5"/>
       <c r="T89" s="5"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B90" s="16"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="E90" s="56" t="n">
+        <v>0.75</v>
+      </c>
       <c r="M90" s="5"/>
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
@@ -2584,6 +2609,17 @@
       <c r="T90" s="5"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91" s="57"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="E91" s="56" t="n">
+        <v>0.75</v>
+      </c>
       <c r="M91" s="5"/>
       <c r="N91" s="5"/>
       <c r="O91" s="5"/>
@@ -2593,12 +2629,7 @@
       <c r="S91" s="5"/>
       <c r="T91" s="5"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5"/>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="M92" s="5"/>
       <c r="N92" s="5"/>
       <c r="O92" s="5"/>
@@ -2609,11 +2640,6 @@
       <c r="T92" s="5"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
       <c r="M93" s="5"/>
       <c r="N93" s="5"/>
       <c r="O93" s="5"/>
@@ -3154,6 +3180,14 @@
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
       <c r="E129" s="5"/>
+      <c r="M129" s="5"/>
+      <c r="N129" s="5"/>
+      <c r="O129" s="5"/>
+      <c r="P129" s="5"/>
+      <c r="Q129" s="5"/>
+      <c r="R129" s="5"/>
+      <c r="S129" s="5"/>
+      <c r="T129" s="5"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="5"/>
@@ -3161,6 +3195,14 @@
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
       <c r="E130" s="5"/>
+      <c r="M130" s="5"/>
+      <c r="N130" s="5"/>
+      <c r="O130" s="5"/>
+      <c r="P130" s="5"/>
+      <c r="Q130" s="5"/>
+      <c r="R130" s="5"/>
+      <c r="S130" s="5"/>
+      <c r="T130" s="5"/>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="5"/>
@@ -4289,13 +4331,25 @@
       <c r="D291" s="5"/>
       <c r="E291" s="5"/>
     </row>
-    <row r="12160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12160" s="56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A292" s="5"/>
+      <c r="B292" s="5"/>
+      <c r="C292" s="5"/>
+      <c r="D292" s="5"/>
+      <c r="E292" s="5"/>
+    </row>
+    <row r="293" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="5"/>
+      <c r="B293" s="5"/>
+      <c r="C293" s="5"/>
+      <c r="D293" s="5"/>
+      <c r="E293" s="5"/>
+    </row>
+    <row r="12162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12162" s="59" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="61">
     <mergeCell ref="A1:E1"/>
@@ -4349,16 +4403,16 @@
     <mergeCell ref="A68:B69"/>
     <mergeCell ref="A70:E70"/>
     <mergeCell ref="C71:E71"/>
-    <mergeCell ref="A76:E76"/>
-    <mergeCell ref="A77:E81"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A78:E78"/>
+    <mergeCell ref="A79:E83"/>
+    <mergeCell ref="A84:E84"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D86:E86"/>
     <mergeCell ref="D87:E87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.354166666666667" bottom="0.354166666666667" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4370,7 +4424,7 @@
   <rowBreaks count="3" manualBreakCount="3">
     <brk id="28" man="true" max="16383" min="0"/>
     <brk id="53" man="true" max="16383" min="0"/>
-    <brk id="88" man="true" max="16383" min="0"/>
+    <brk id="90" man="true" max="16383" min="0"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -4390,7 +4444,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="57" width="28.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="28.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.4"/>
@@ -4402,87 +4456,87 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7"/>
-      <c r="C2" s="57" t="n">
+      <c r="C2" s="60" t="n">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
-      <c r="C3" s="57" t="n">
+      <c r="C3" s="60" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
-      <c r="C4" s="57" t="n">
+      <c r="C4" s="60" t="n">
         <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
-      <c r="C5" s="57" t="n">
+      <c r="C5" s="60" t="n">
         <v>4</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
-      <c r="C6" s="57" t="n">
+      <c r="C6" s="60" t="n">
         <v>5</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
-      <c r="C7" s="57" t="n">
+      <c r="C7" s="60" t="n">
         <v>6</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
-      <c r="C8" s="57" t="n">
+      <c r="C8" s="60" t="n">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="57" t="n">
+      <c r="B9" s="61"/>
+      <c r="C9" s="60" t="n">
         <v>8</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
-      <c r="C10" s="57" t="s">
-        <v>112</v>
+      <c r="C10" s="60" t="s">
+        <v>115</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G10" s="0" t="n">
         <v>1</v>
@@ -4493,14 +4547,14 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
-      <c r="C12" s="57" t="s">
-        <v>115</v>
+      <c r="C12" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G12" s="0" t="n">
         <v>3</v>
@@ -4509,10 +4563,10 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
       <c r="E13" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>5</v>
@@ -4521,7 +4575,7 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="E14" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>7</v>
@@ -4535,18 +4589,18 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7"/>
-      <c r="B16" s="58"/>
+      <c r="B16" s="61"/>
       <c r="G16" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
-      <c r="C17" s="57" t="s">
-        <v>115</v>
+      <c r="C17" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G17" s="0" t="n">
         <v>10</v>
@@ -4554,11 +4608,11 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
-      <c r="C18" s="57" t="s">
-        <v>115</v>
+      <c r="C18" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G18" s="0" t="n">
         <v>11</v>
@@ -4566,281 +4620,281 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7"/>
-      <c r="C19" s="57" t="s">
-        <v>115</v>
+      <c r="C19" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G19" s="0" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="59"/>
-      <c r="C20" s="57" t="s">
-        <v>115</v>
+      <c r="A20" s="62"/>
+      <c r="C20" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="59"/>
-      <c r="C21" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="60" t="s">
-        <v>125</v>
+      <c r="A21" s="62"/>
+      <c r="C21" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="63" t="s">
+        <v>128</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="59"/>
-      <c r="C22" s="57" t="s">
-        <v>115</v>
+      <c r="A22" s="62"/>
+      <c r="C22" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G22" s="0" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="59"/>
-      <c r="C23" s="57" t="s">
-        <v>115</v>
+      <c r="A23" s="62"/>
+      <c r="C23" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G23" s="0" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="59"/>
-      <c r="C24" s="57" t="s">
-        <v>115</v>
+      <c r="A24" s="62"/>
+      <c r="C24" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G24" s="0" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="59"/>
-      <c r="C25" s="57" t="s">
-        <v>129</v>
+      <c r="A25" s="62"/>
+      <c r="C25" s="60" t="s">
+        <v>132</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="G25" s="60" t="n">
+        <v>133</v>
+      </c>
+      <c r="G25" s="63" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="59"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="57" t="s">
-        <v>115</v>
+      <c r="C26" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="G26" s="60" t="n">
+        <v>134</v>
+      </c>
+      <c r="G26" s="63" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="59"/>
-      <c r="B27" s="61" t="s">
-        <v>132</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>115</v>
+      <c r="A27" s="62"/>
+      <c r="B27" s="64" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="G27" s="60" t="n">
+        <v>136</v>
+      </c>
+      <c r="G27" s="63" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="59"/>
-      <c r="B28" s="62" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="57" t="s">
-        <v>115</v>
+      <c r="A28" s="62"/>
+      <c r="B28" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="60" t="s">
+        <v>118</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G28" s="60" t="n">
+        <v>138</v>
+      </c>
+      <c r="G28" s="63" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="59"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="64" t="s">
-        <v>115</v>
+      <c r="A29" s="62"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="67" t="s">
+        <v>118</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="60" t="n">
+        <v>139</v>
+      </c>
+      <c r="G29" s="63" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="59"/>
-      <c r="B30" s="63" t="n">
+      <c r="A30" s="62"/>
+      <c r="B30" s="66" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="64" t="s">
-        <v>115</v>
+      <c r="C30" s="67" t="s">
+        <v>118</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="60" t="n">
+        <v>140</v>
+      </c>
+      <c r="G30" s="63" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="59"/>
-      <c r="B31" s="63" t="n">
+      <c r="A31" s="62"/>
+      <c r="B31" s="66" t="n">
         <v>2</v>
       </c>
-      <c r="C31" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="E31" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60" t="n">
+      <c r="C31" s="67" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="59"/>
-      <c r="B32" s="63" t="n">
+      <c r="A32" s="62"/>
+      <c r="B32" s="66" t="n">
         <v>3</v>
       </c>
-      <c r="C32" s="64" t="s">
-        <v>115</v>
+      <c r="C32" s="67" t="s">
+        <v>118</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="F32" s="60"/>
-      <c r="G32" s="63" t="n">
+        <v>142</v>
+      </c>
+      <c r="F32" s="63"/>
+      <c r="G32" s="66" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="59"/>
-      <c r="B33" s="63" t="n">
+      <c r="A33" s="62"/>
+      <c r="B33" s="66" t="n">
         <v>4</v>
       </c>
-      <c r="C33" s="64" t="s">
-        <v>115</v>
+      <c r="C33" s="67" t="s">
+        <v>118</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="E33" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33" s="60"/>
-      <c r="G33" s="63" t="n">
+        <v>143</v>
+      </c>
+      <c r="E33" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="63"/>
+      <c r="G33" s="66" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="59"/>
-      <c r="B34" s="63" t="n">
+      <c r="A34" s="62"/>
+      <c r="B34" s="66" t="n">
         <v>5</v>
       </c>
-      <c r="C34" s="64" t="s">
-        <v>115</v>
+      <c r="C34" s="67" t="s">
+        <v>118</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34" s="60"/>
-      <c r="G34" s="63" t="n">
+        <v>118</v>
+      </c>
+      <c r="F34" s="63"/>
+      <c r="G34" s="66" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="59"/>
-      <c r="B35" s="63" t="n">
+      <c r="A35" s="62"/>
+      <c r="B35" s="66" t="n">
         <v>6</v>
       </c>
-      <c r="C35" s="64" t="s">
-        <v>115</v>
+      <c r="C35" s="67" t="s">
+        <v>118</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="63" t="n">
+        <v>144</v>
+      </c>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="66" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="63" t="n">
+      <c r="B36" s="66" t="n">
         <v>7</v>
       </c>
-      <c r="C36" s="65" t="s">
-        <v>115</v>
+      <c r="C36" s="68" t="s">
+        <v>118</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>31</v>
       </c>
       <c r="E36" s="5"/>
-      <c r="G36" s="63" t="n">
+      <c r="G36" s="66" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
-      <c r="B37" s="63" t="n">
+      <c r="B37" s="66" t="n">
         <v>8</v>
       </c>
-      <c r="C37" s="65" t="s">
-        <v>115</v>
+      <c r="C37" s="68" t="s">
+        <v>118</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="E37" s="5"/>
-      <c r="G37" s="63" t="n">
+      <c r="G37" s="66" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
-      <c r="B38" s="63" t="n">
+      <c r="B38" s="66" t="n">
         <v>9</v>
       </c>
-      <c r="C38" s="65" t="s">
-        <v>115</v>
+      <c r="C38" s="68" t="s">
+        <v>118</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -4849,8 +4903,8 @@
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="65" t="s">
-        <v>115</v>
+      <c r="C39" s="68" t="s">
+        <v>118</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>38</v>
@@ -4866,7 +4920,7 @@
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -4875,11 +4929,11 @@
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="5" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -4888,10 +4942,10 @@
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="31"/>
       <c r="B42" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="C42" s="66"/>
-      <c r="D42" s="67"/>
+        <v>118</v>
+      </c>
+      <c r="C42" s="69"/>
+      <c r="D42" s="70"/>
       <c r="E42" s="31"/>
       <c r="F42" s="31"/>
       <c r="G42" s="31"/>
@@ -4899,10 +4953,10 @@
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
       <c r="B43" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C43" s="8"/>
-      <c r="D43" s="60"/>
+      <c r="D43" s="63"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -4911,29 +4965,29 @@
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="8"/>
-      <c r="D44" s="60"/>
+      <c r="D44" s="63"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5"/>
-      <c r="B45" s="62" t="s">
+      <c r="B45" s="65" t="s">
         <v>27</v>
       </c>
       <c r="C45" s="8"/>
-      <c r="D45" s="60"/>
+      <c r="D45" s="63"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5"/>
-      <c r="B46" s="68" t="s">
-        <v>143</v>
+      <c r="B46" s="71" t="s">
+        <v>146</v>
       </c>
       <c r="C46" s="8"/>
-      <c r="D46" s="60"/>
+      <c r="D46" s="63"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -4942,32 +4996,32 @@
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="8"/>
-      <c r="D47" s="60"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5"/>
-      <c r="B48" s="69" t="s">
-        <v>146</v>
-      </c>
-      <c r="C48" s="69" t="s">
-        <v>147</v>
-      </c>
-      <c r="E48" s="70" t="s">
+      <c r="B48" s="72" t="s">
+        <v>149</v>
+      </c>
+      <c r="C48" s="72" t="s">
+        <v>150</v>
+      </c>
+      <c r="E48" s="73" t="s">
         <v>32</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="62" t="s">
-        <v>115</v>
+      <c r="B49" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -4977,17 +5031,17 @@
       <c r="B50" s="5"/>
       <c r="C50" s="8"/>
       <c r="D50" s="5" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E50" s="5"/>
-      <c r="F50" s="70"/>
+      <c r="F50" s="73"/>
       <c r="G50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="5"/>
       <c r="C51" s="8"/>
       <c r="D51" s="5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -4996,8 +5050,8 @@
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="5"/>
       <c r="C52" s="8"/>
-      <c r="D52" s="62" t="s">
-        <v>115</v>
+      <c r="D52" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -5023,15 +5077,15 @@
       <c r="B55" s="5"/>
       <c r="C55" s="8"/>
       <c r="D55" s="5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="71" t="s">
-        <v>152</v>
+      <c r="B56" s="74" t="s">
+        <v>155</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>50</v>
@@ -5040,7 +5094,7 @@
         <v>29</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
@@ -5050,99 +5104,99 @@
         <v>31</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>153</v>
+        <v>94</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="62" t="s">
-        <v>155</v>
+      <c r="B59" s="65" t="s">
+        <v>157</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="D59" s="62" t="s">
-        <v>153</v>
-      </c>
-      <c r="E59" s="62" t="s">
-        <v>115</v>
+        <v>158</v>
+      </c>
+      <c r="D59" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="62"/>
+      <c r="B60" s="65"/>
       <c r="C60" s="8"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="62"/>
+      <c r="E60" s="65"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="5"/>
       <c r="C61" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D61" s="62" t="s">
-        <v>115</v>
-      </c>
-      <c r="E61" s="62" t="s">
-        <v>115</v>
+        <v>159</v>
+      </c>
+      <c r="D61" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E61" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="72" t="s">
+      <c r="B62" s="75" t="s">
         <v>30</v>
       </c>
       <c r="C62" s="8"/>
-      <c r="D62" s="69" t="s">
-        <v>158</v>
+      <c r="D62" s="72" t="s">
+        <v>160</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="73" t="s">
-        <v>159</v>
+      <c r="B63" s="76" t="s">
+        <v>161</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D63" s="62" t="s">
-        <v>115</v>
+      <c r="D63" s="65" t="s">
+        <v>118</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="72" t="s">
-        <v>160</v>
+      <c r="B64" s="75" t="s">
+        <v>162</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>153</v>
+        <v>94</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
@@ -5150,10 +5204,10 @@
       <c r="G64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="67"/>
-      <c r="B65" s="74"/>
-      <c r="C65" s="66" t="s">
-        <v>155</v>
+      <c r="A65" s="70"/>
+      <c r="B65" s="77"/>
+      <c r="C65" s="69" t="s">
+        <v>157</v>
       </c>
       <c r="D65" s="31"/>
       <c r="E65" s="31"/>
@@ -5185,9 +5239,9 @@
       <c r="G68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="67"/>
+      <c r="A69" s="70"/>
       <c r="B69" s="31"/>
-      <c r="C69" s="66"/>
+      <c r="C69" s="69"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
       <c r="F69" s="31"/>
@@ -5196,8 +5250,8 @@
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="5"/>
       <c r="C70" s="8"/>
-      <c r="D70" s="72" t="s">
-        <v>115</v>
+      <c r="D70" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -5205,12 +5259,12 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B71" s="5"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="72" t="s">
-        <v>115</v>
+      <c r="D71" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
@@ -5222,19 +5276,19 @@
       </c>
       <c r="B72" s="5"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="72" t="s">
-        <v>115</v>
+      <c r="D72" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="62"/>
+      <c r="A73" s="65"/>
       <c r="B73" s="5"/>
       <c r="C73" s="8"/>
-      <c r="D73" s="72" t="s">
-        <v>115</v>
+      <c r="D73" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -5246,8 +5300,8 @@
       </c>
       <c r="B74" s="5"/>
       <c r="C74" s="8"/>
-      <c r="D74" s="72" t="s">
-        <v>115</v>
+      <c r="D74" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -5256,7 +5310,7 @@
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="5"/>
       <c r="C75" s="8"/>
-      <c r="D75" s="72"/>
+      <c r="D75" s="75"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
@@ -5264,32 +5318,32 @@
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="5"/>
       <c r="C76" s="8"/>
-      <c r="D76" s="72" t="s">
-        <v>115</v>
+      <c r="D76" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="62" t="s">
+      <c r="A77" s="65" t="s">
         <v>72</v>
       </c>
       <c r="B77" s="5"/>
       <c r="C77" s="8"/>
-      <c r="D77" s="72" t="s">
-        <v>162</v>
+      <c r="D77" s="75" t="s">
+        <v>164</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="62"/>
+      <c r="A78" s="65"/>
       <c r="B78" s="5"/>
       <c r="C78" s="8"/>
-      <c r="D78" s="72" t="s">
-        <v>115</v>
+      <c r="D78" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
@@ -5298,8 +5352,8 @@
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="5"/>
       <c r="C79" s="8"/>
-      <c r="D79" s="72" t="s">
-        <v>115</v>
+      <c r="D79" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
@@ -5308,8 +5362,8 @@
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="5"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="72" t="s">
-        <v>115</v>
+      <c r="D80" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
@@ -5318,8 +5372,8 @@
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="5"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="72" t="s">
-        <v>115</v>
+      <c r="D81" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
@@ -5328,8 +5382,8 @@
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="5"/>
       <c r="C82" s="8"/>
-      <c r="D82" s="72" t="s">
-        <v>115</v>
+      <c r="D82" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
@@ -5338,8 +5392,8 @@
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="5"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="72" t="s">
-        <v>115</v>
+      <c r="D83" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
@@ -5348,186 +5402,186 @@
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="5"/>
       <c r="C84" s="8"/>
-      <c r="D84" s="72" t="s">
-        <v>115</v>
+      <c r="D84" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
-      <c r="G84" s="72" t="n">
+      <c r="G84" s="75" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="5"/>
       <c r="C85" s="8"/>
-      <c r="D85" s="72"/>
+      <c r="D85" s="75"/>
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
-      <c r="G85" s="72" t="n">
+      <c r="G85" s="75" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="5"/>
       <c r="C86" s="8"/>
-      <c r="D86" s="72"/>
+      <c r="D86" s="75"/>
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
-      <c r="G86" s="72" t="n">
+      <c r="G86" s="75" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="5"/>
       <c r="C87" s="8"/>
-      <c r="D87" s="72" t="s">
-        <v>115</v>
+      <c r="D87" s="75" t="s">
+        <v>118</v>
       </c>
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
-      <c r="G87" s="72" t="n">
+      <c r="G87" s="75" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B88" s="5"/>
       <c r="C88" s="8"/>
-      <c r="D88" s="72"/>
-      <c r="E88" s="57" t="n">
+      <c r="D88" s="75"/>
+      <c r="E88" s="60" t="n">
         <v>0</v>
       </c>
       <c r="F88" s="5"/>
-      <c r="G88" s="72" t="n">
+      <c r="G88" s="75" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="5"/>
       <c r="C89" s="8"/>
-      <c r="D89" s="72"/>
-      <c r="E89" s="57" t="n">
+      <c r="D89" s="75"/>
+      <c r="E89" s="60" t="n">
         <v>1</v>
       </c>
       <c r="F89" s="5"/>
-      <c r="G89" s="72" t="n">
+      <c r="G89" s="75" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B90" s="5"/>
       <c r="C90" s="8"/>
-      <c r="D90" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="E90" s="57" t="n">
+      <c r="D90" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="E90" s="60" t="n">
         <v>1.5</v>
       </c>
       <c r="F90" s="5"/>
-      <c r="G90" s="72" t="n">
+      <c r="G90" s="75" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B91" s="5"/>
       <c r="C91" s="8"/>
-      <c r="D91" s="72"/>
-      <c r="E91" s="57" t="n">
+      <c r="D91" s="75"/>
+      <c r="E91" s="60" t="n">
         <v>2</v>
       </c>
       <c r="F91" s="5"/>
-      <c r="G91" s="72" t="n">
+      <c r="G91" s="75" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B92" s="5"/>
       <c r="C92" s="8"/>
-      <c r="D92" s="72"/>
-      <c r="E92" s="57" t="n">
+      <c r="D92" s="75"/>
+      <c r="E92" s="60" t="n">
         <v>2</v>
       </c>
       <c r="F92" s="5"/>
-      <c r="G92" s="72" t="n">
+      <c r="G92" s="75" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B93" s="5"/>
       <c r="C93" s="8"/>
-      <c r="D93" s="72"/>
-      <c r="E93" s="57" t="n">
+      <c r="D93" s="75"/>
+      <c r="E93" s="60" t="n">
         <v>3</v>
       </c>
       <c r="F93" s="5"/>
-      <c r="G93" s="72" t="n">
+      <c r="G93" s="75" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="5"/>
       <c r="C94" s="8"/>
-      <c r="D94" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="E94" s="57" t="n">
+      <c r="D94" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="E94" s="60" t="n">
         <v>3.5</v>
       </c>
       <c r="F94" s="5"/>
-      <c r="G94" s="72" t="n">
+      <c r="G94" s="75" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="5"/>
       <c r="C95" s="8"/>
-      <c r="D95" s="72"/>
-      <c r="E95" s="57" t="n">
+      <c r="D95" s="75"/>
+      <c r="E95" s="60" t="n">
         <v>4</v>
       </c>
       <c r="F95" s="5"/>
-      <c r="G95" s="72" t="n">
+      <c r="G95" s="75" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="5"/>
       <c r="C96" s="8"/>
-      <c r="D96" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="E96" s="57" t="n">
+      <c r="D96" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="E96" s="60" t="n">
         <v>4.5</v>
       </c>
       <c r="F96" s="5"/>
-      <c r="G96" s="72" t="n">
+      <c r="G96" s="75" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="5"/>
       <c r="C97" s="8"/>
-      <c r="D97" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="E97" s="57" t="n">
+      <c r="D97" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="E97" s="60" t="n">
         <v>5</v>
       </c>
       <c r="F97" s="5"/>
-      <c r="G97" s="72" t="n">
+      <c r="G97" s="75" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="5"/>
       <c r="C98" s="8"/>
-      <c r="D98" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="E98" s="57" t="n">
+      <c r="D98" s="75" t="s">
+        <v>118</v>
+      </c>
+      <c r="E98" s="60" t="n">
         <v>5.5</v>
       </c>
       <c r="F98" s="5"/>
-      <c r="G98" s="72" t="n">
+      <c r="G98" s="75" t="n">
         <v>15</v>
       </c>
     </row>
@@ -5535,11 +5589,11 @@
       <c r="B99" s="5"/>
       <c r="C99" s="8"/>
       <c r="D99" s="5"/>
-      <c r="E99" s="57" t="n">
+      <c r="E99" s="60" t="n">
         <v>6</v>
       </c>
       <c r="F99" s="5"/>
-      <c r="G99" s="72" t="n">
+      <c r="G99" s="75" t="n">
         <v>16</v>
       </c>
     </row>
@@ -5547,11 +5601,11 @@
       <c r="B100" s="5"/>
       <c r="C100" s="8"/>
       <c r="D100" s="5"/>
-      <c r="E100" s="57" t="n">
+      <c r="E100" s="60" t="n">
         <v>6.5</v>
       </c>
       <c r="F100" s="5"/>
-      <c r="G100" s="72" t="n">
+      <c r="G100" s="75" t="n">
         <v>17</v>
       </c>
     </row>
@@ -5559,51 +5613,51 @@
       <c r="B101" s="5"/>
       <c r="C101" s="8"/>
       <c r="D101" s="5"/>
-      <c r="E101" s="57" t="n">
+      <c r="E101" s="60" t="n">
         <v>7</v>
       </c>
       <c r="F101" s="5"/>
-      <c r="G101" s="72" t="n">
+      <c r="G101" s="75" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B102" s="5"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="75"/>
-      <c r="E102" s="57" t="n">
+      <c r="D102" s="78"/>
+      <c r="E102" s="60" t="n">
         <v>7.5</v>
       </c>
       <c r="F102" s="5"/>
-      <c r="G102" s="72" t="n">
+      <c r="G102" s="75" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="5"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="76" t="s">
+      <c r="D103" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="E103" s="57" t="n">
+      <c r="E103" s="60" t="n">
         <v>8</v>
       </c>
       <c r="F103" s="5"/>
-      <c r="G103" s="72" t="n">
+      <c r="G103" s="75" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="5"/>
       <c r="C104" s="8"/>
-      <c r="D104" s="76" t="s">
-        <v>153</v>
-      </c>
-      <c r="E104" s="57" t="n">
+      <c r="D104" s="79" t="s">
+        <v>94</v>
+      </c>
+      <c r="E104" s="60" t="n">
         <v>8.5</v>
       </c>
       <c r="F104" s="5"/>
-      <c r="G104" s="72" t="n">
+      <c r="G104" s="75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5611,37 +5665,37 @@
       <c r="B105" s="5"/>
       <c r="C105" s="8"/>
       <c r="D105" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E105" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E105" s="60" t="n">
         <v>9</v>
       </c>
       <c r="F105" s="5"/>
-      <c r="G105" s="72" t="s">
-        <v>115</v>
+      <c r="G105" s="75" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="5"/>
       <c r="C106" s="8"/>
       <c r="D106" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E106" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E106" s="60" t="n">
         <v>9.5</v>
       </c>
       <c r="F106" s="5"/>
-      <c r="G106" s="72" t="s">
-        <v>115</v>
+      <c r="G106" s="75" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="5"/>
       <c r="C107" s="8"/>
       <c r="D107" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E107" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E107" s="60" t="n">
         <v>10</v>
       </c>
       <c r="F107" s="5"/>
@@ -5651,9 +5705,9 @@
       <c r="B108" s="5"/>
       <c r="C108" s="8"/>
       <c r="D108" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E108" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E108" s="60" t="n">
         <v>10.5</v>
       </c>
       <c r="F108" s="5"/>
@@ -5662,7 +5716,7 @@
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="5"/>
       <c r="C109" s="8"/>
-      <c r="E109" s="57" t="n">
+      <c r="E109" s="60" t="n">
         <v>11</v>
       </c>
       <c r="F109" s="5"/>
@@ -5671,7 +5725,7 @@
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B110" s="5"/>
       <c r="C110" s="8"/>
-      <c r="E110" s="57" t="n">
+      <c r="E110" s="60" t="n">
         <v>11.5</v>
       </c>
       <c r="F110" s="5"/>
@@ -5681,9 +5735,9 @@
       <c r="B111" s="5"/>
       <c r="C111" s="8"/>
       <c r="D111" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E111" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E111" s="60" t="n">
         <v>12</v>
       </c>
       <c r="F111" s="5"/>
@@ -5693,9 +5747,9 @@
       <c r="B112" s="5"/>
       <c r="C112" s="8"/>
       <c r="D112" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E112" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E112" s="60" t="n">
         <v>12.5</v>
       </c>
       <c r="F112" s="5"/>
@@ -5705,9 +5759,9 @@
       <c r="B113" s="5"/>
       <c r="C113" s="8"/>
       <c r="D113" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E113" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E113" s="60" t="n">
         <v>13</v>
       </c>
       <c r="F113" s="5"/>
@@ -5717,9 +5771,9 @@
       <c r="B114" s="5"/>
       <c r="C114" s="8"/>
       <c r="D114" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E114" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E114" s="60" t="n">
         <v>13.5</v>
       </c>
       <c r="F114" s="5"/>
@@ -5728,10 +5782,10 @@
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="5"/>
       <c r="C115" s="8"/>
-      <c r="D115" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="E115" s="57" t="n">
+      <c r="D115" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E115" s="60" t="n">
         <v>14</v>
       </c>
       <c r="F115" s="5"/>
@@ -5741,9 +5795,9 @@
       <c r="B116" s="5"/>
       <c r="C116" s="8"/>
       <c r="D116" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E116" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E116" s="60" t="n">
         <v>14.5</v>
       </c>
       <c r="F116" s="5"/>
@@ -5753,9 +5807,9 @@
       <c r="B117" s="5"/>
       <c r="C117" s="8"/>
       <c r="D117" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E117" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E117" s="60" t="n">
         <v>15</v>
       </c>
       <c r="F117" s="5"/>
@@ -5765,9 +5819,9 @@
       <c r="B118" s="5"/>
       <c r="C118" s="8"/>
       <c r="D118" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E118" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E118" s="60" t="n">
         <v>15.5</v>
       </c>
       <c r="F118" s="5"/>
@@ -5777,9 +5831,9 @@
       <c r="B119" s="5"/>
       <c r="C119" s="8"/>
       <c r="D119" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E119" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E119" s="60" t="n">
         <v>16</v>
       </c>
       <c r="F119" s="5"/>
@@ -5789,9 +5843,9 @@
       <c r="B120" s="5"/>
       <c r="C120" s="8"/>
       <c r="D120" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E120" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E120" s="60" t="n">
         <v>16.5</v>
       </c>
       <c r="F120" s="5"/>
@@ -5801,9 +5855,9 @@
       <c r="B121" s="5"/>
       <c r="C121" s="8"/>
       <c r="D121" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E121" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E121" s="60" t="n">
         <v>17</v>
       </c>
       <c r="F121" s="5"/>
@@ -5813,9 +5867,9 @@
       <c r="B122" s="5"/>
       <c r="C122" s="8"/>
       <c r="D122" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E122" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E122" s="60" t="n">
         <v>17.5</v>
       </c>
       <c r="F122" s="5"/>
@@ -5825,9 +5879,9 @@
       <c r="B123" s="5"/>
       <c r="C123" s="8"/>
       <c r="D123" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E123" s="57" t="n">
+        <v>118</v>
+      </c>
+      <c r="E123" s="60" t="n">
         <v>18</v>
       </c>
       <c r="F123" s="5"/>
@@ -5836,10 +5890,10 @@
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B124" s="5"/>
       <c r="C124" s="8"/>
-      <c r="D124" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="E124" s="57" t="n">
+      <c r="D124" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E124" s="60" t="n">
         <v>18.5</v>
       </c>
       <c r="F124" s="5"/>
@@ -5849,9 +5903,9 @@
       <c r="B125" s="5"/>
       <c r="C125" s="8"/>
       <c r="D125" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E125" s="64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E125" s="67" t="n">
         <v>19</v>
       </c>
       <c r="F125" s="5"/>
@@ -5861,9 +5915,9 @@
       <c r="B126" s="5"/>
       <c r="C126" s="8"/>
       <c r="D126" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E126" s="64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E126" s="67" t="n">
         <v>19.5</v>
       </c>
       <c r="F126" s="5"/>
@@ -5873,9 +5927,9 @@
       <c r="B127" s="5"/>
       <c r="C127" s="8"/>
       <c r="D127" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E127" s="64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E127" s="67" t="n">
         <v>20</v>
       </c>
       <c r="F127" s="5"/>
@@ -5885,9 +5939,9 @@
       <c r="B128" s="5"/>
       <c r="C128" s="8"/>
       <c r="D128" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E128" s="64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E128" s="67" t="n">
         <v>20.5</v>
       </c>
       <c r="F128" s="5"/>
@@ -5897,9 +5951,9 @@
       <c r="B129" s="5"/>
       <c r="C129" s="8"/>
       <c r="D129" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E129" s="64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E129" s="67" t="n">
         <v>21</v>
       </c>
       <c r="F129" s="5"/>
@@ -5909,9 +5963,9 @@
       <c r="B130" s="5"/>
       <c r="C130" s="8"/>
       <c r="D130" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E130" s="64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E130" s="67" t="n">
         <v>21.5</v>
       </c>
       <c r="F130" s="5"/>
@@ -5921,9 +5975,9 @@
       <c r="B131" s="5"/>
       <c r="C131" s="8"/>
       <c r="D131" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E131" s="64" t="n">
+        <v>118</v>
+      </c>
+      <c r="E131" s="67" t="n">
         <v>22</v>
       </c>
       <c r="F131" s="5"/>
@@ -5933,9 +5987,9 @@
       <c r="B132" s="5"/>
       <c r="C132" s="8"/>
       <c r="D132" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E132" s="65" t="n">
+        <v>118</v>
+      </c>
+      <c r="E132" s="68" t="n">
         <v>22.5</v>
       </c>
       <c r="F132" s="5"/>
@@ -5945,9 +5999,9 @@
       <c r="B133" s="5"/>
       <c r="C133" s="8"/>
       <c r="D133" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E133" s="65" t="n">
+        <v>118</v>
+      </c>
+      <c r="E133" s="68" t="n">
         <v>23</v>
       </c>
       <c r="F133" s="5"/>
@@ -5956,10 +6010,10 @@
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B134" s="5"/>
       <c r="C134" s="8"/>
-      <c r="D134" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="E134" s="65" t="n">
+      <c r="D134" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E134" s="68" t="n">
         <v>23.5</v>
       </c>
       <c r="F134" s="5"/>
@@ -5969,9 +6023,9 @@
       <c r="B135" s="5"/>
       <c r="C135" s="8"/>
       <c r="D135" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="E135" s="65" t="n">
+        <v>118</v>
+      </c>
+      <c r="E135" s="68" t="n">
         <v>24</v>
       </c>
       <c r="F135" s="5"/>
@@ -5980,9 +6034,9 @@
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B136" s="5"/>
       <c r="C136" s="8"/>
-      <c r="D136" s="60"/>
-      <c r="E136" s="65" t="s">
-        <v>115</v>
+      <c r="D136" s="63"/>
+      <c r="E136" s="68" t="s">
+        <v>118</v>
       </c>
       <c r="F136" s="5"/>
       <c r="G136" s="5"/>
@@ -5991,8 +6045,8 @@
       <c r="B137" s="5"/>
       <c r="C137" s="8"/>
       <c r="D137" s="5"/>
-      <c r="E137" s="65" t="s">
-        <v>115</v>
+      <c r="E137" s="68" t="s">
+        <v>118</v>
       </c>
       <c r="F137" s="5"/>
       <c r="G137" s="5"/>
@@ -6169,141 +6223,141 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="77"/>
+      <c r="C3" s="80"/>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="79" t="s">
-        <v>163</v>
+      <c r="E4" s="82" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="80" t="s">
-        <v>164</v>
-      </c>
-      <c r="E5" s="72" t="s">
+      <c r="C5" s="83" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="81" t="s">
-        <v>165</v>
+      <c r="G5" s="84" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="80" t="s">
-        <v>166</v>
-      </c>
-      <c r="E6" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="81" t="s">
-        <v>167</v>
+      <c r="C6" s="83" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="84" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="80" t="s">
-        <v>168</v>
-      </c>
-      <c r="E7" s="72" t="s">
-        <v>160</v>
+      <c r="C7" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="E7" s="75" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="80" t="s">
-        <v>169</v>
+      <c r="C8" s="83" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="80" t="s">
-        <v>170</v>
+      <c r="C9" s="83" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="80" t="s">
-        <v>171</v>
+      <c r="C10" s="83" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="82" t="s">
-        <v>172</v>
+      <c r="C11" s="85" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="80" t="s">
-        <v>173</v>
+      <c r="C12" s="83" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="80" t="s">
-        <v>174</v>
+      <c r="C13" s="83" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="80" t="s">
-        <v>175</v>
+      <c r="C14" s="83" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="80" t="s">
-        <v>176</v>
+      <c r="C15" s="83" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="80" t="s">
-        <v>177</v>
+      <c r="C16" s="83" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="80" t="s">
-        <v>178</v>
+      <c r="C17" s="83" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="82" t="s">
-        <v>155</v>
+      <c r="C18" s="85" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="80" t="s">
-        <v>179</v>
+      <c r="C19" s="83" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="80" t="s">
-        <v>180</v>
+      <c r="C20" s="83" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="80" t="s">
-        <v>181</v>
+      <c r="C21" s="83" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="80" t="s">
-        <v>182</v>
+      <c r="C22" s="83" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="80" t="s">
-        <v>183</v>
+      <c r="C23" s="83" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="80" t="s">
-        <v>184</v>
+      <c r="C24" s="83" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="83" t="s">
-        <v>185</v>
+      <c r="C25" s="86" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="84"/>
+      <c r="C26" s="87"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="84"/>
+      <c r="C27" s="87"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>